<commit_message>
Added class Data, installed System.Text.JSON plus System.Text.SQLClient and Create Database
</commit_message>
<xml_diff>
--- a/ClientDictApp/Records/records.xlsx
+++ b/ClientDictApp/Records/records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\network_programming_midterm\Records\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD5CDDA-EBF1-4F3B-82D2-E6A54C8310D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4210534-5AC5-4CBC-847B-05CBC55C9BE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5317" yWindow="3733" windowWidth="15951" windowHeight="8230" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
   <si>
     <t>Encoded word</t>
   </si>
@@ -1322,6 +1322,128 @@
 - đưa (đội bóng) ra sân
 *  nội động từ
 - (thể dục,thể thao) làm người chặn bóng (crickê)
+</t>
+  </si>
+  <si>
+    <t>ace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@ace /eis/
+*  danh từ
+- (đánh bài) quân át, quân xì; điểm 1 (trên quân bài hay con súc sắc)
+=duece ace+ một con "hai" và một con "một" (đánh súc sắc)
+- phi công xuất sắc (hạ được trên mười máy bay địch); vận động viên xuất sắc; người giỏi nhất (về cái gì...); nhà vô địch
+- (thể dục,thể thao) cú giao bóng thắng điểm; điểm thắng giao bóng (quần vợt)
+- chút xíu
+=to be within an ace of death+ suýt nữa thì chết
+!ace in the hole
+- (từ Mỹ,nghĩa Mỹ),  (thông tục) quân bài chủ cao nhất dành cho lúc cần đến (đen &amp; bóng)
+- người bạn có thể dựa khi gặp khó khăn
+!the ace of aces
+- phi công ưu tú nhất
+- người xuất sắc nhất trong những người xuất sắc
+!the ace of trumps
+- quân bài chủ cao nhất
+!to have an ace up one's sleeve
+- giữ kín quân bài chủ cao nhất dành cho lúc cần
+!to trump somebody's ace
+- cắt quân át của ai bằng bài chủ
+- gạt được một đòn ác hiểm của ai
+</t>
+  </si>
+  <si>
+    <t>she</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@she /ʃi:/
+*  đại từ
+- nó, bà ấy, chị ấy, cô ấy...
+=she sings beautifully+ chị ấy hát hay
+- nó (chỉ tàu, xe... đã được nhân cách hoá), tàu ấy, xe ấy
+=she sails tomorrow+ ngày mai chiếc tàu ấy nhổ neo
+- người đàn bà, chị
+=she of the black hair+ người đàn bà tóc đen, chị tóc đen
+*  danh từ
+- đàn bà, con gái
+=is the child a he or a she?+ đứa bé là con trai hay con gái?
+=the not impossible she+ người có thể yêu được
+- con cái
+=a litter of two shes and a he+ một ổ hai con cái và một con đực
+- (trong từ ghép chỉ động vật) cái
+=she-goat+ dê cái
+=she-ass+ lừa cái
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@young /jʌɳ/
+*  tính từ
+- trẻ, trẻ tuổi, thiếu niên, thanh niên
+=a young man+ một thanh niên
+=young people+ thanh niên
+=his (her) young woman (man)+ người yêu của nó
+=a young family+ gia đình có nhiều con nhỏ
+=a young person+ người đàn bà lạ trẻ tuổi thuộc tầng lớp dưới (trong ngôn ngữ những người ở của các gia đình tư sản quý tộc Anh)
+=the young person+ những người còn non trẻ ngây thơ cần giữ gìn không cho nghe (đọc) những điều tục tĩu
+- non
+=young tree+ cây non
+- (nghĩa bóng) non trẻ, trẻ tuổi
+=a young republic+ nước cộng hoà trẻ tuổi
+=he is young for his age+ nó còn non so với tuổi, nó trẻ hơn tuổi
+- (nghĩa bóng) non nớt, mới mẻ, chưa có kinh nghiệm
+=young in mind+ trí óc còn non nớt
+=young in bussiness+ chưa có kinh nghiệm kinh doanh
+- (nghĩa bóng) còn sớm, còn ở lúc ban đầu, chưa muộn, chưa quá, chưa già
+=the night is young yet+ đêm chưa khuya
+=young moon+ trăng non
+=autumn is still young+ thu hãy còn đang ở lúc đầu mùa
+- của tuổi trẻ, của thời thanh niên, của thời niên thiếu, (thuộc) thế hệ trẻ
+=young hope+ hy vọng của tuổi trẻ
+=in one's young days+ trong thời kỳ thanh xuân, trong lúc tuổi còn trẻ
+- (thông tục) con, nhỏ
+=young Smith+ thằng Xmít con, cậu Xmít
+*  danh từ
+- thú con, chim con (mới đẻ)
+=with young+ có chửa (thú)
+</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@rose /rouz/
+*  danh từ
+- hoa hồng; cây hoa hồng
+=a climbing rose+ cây hồng leo
+=wild rose+ cây tầm xuân
+- cô gái đẹp nhất, hoa khôi
+=the rose of the town+ cô gái đẹp nhất tỉnh, hoa khôi của tỉnh
+- bông hồng năm cánh (quốc huy của nước Anh)
+- màu hồng; (số nhiều) nước da hồng hào
+=to have roses in one's cheeks+ má đỏ hồng hào
+- nơ hoa hồng (đính ở mũ, ở giầy...)
+- hương sen (bình tưới)
+- (như) rose-diamond
+- (như) rose_window
+- chân sừng (phần lồi lên ở gốc sừng nai, hươu...)
+- (y học) (the rose) bệnh viêm quầng
+=a bed of roses x bed to be born under the rose+ đẻ hoang
+=blue rose+ "bông hồng xanh" (cái không thể nào có được)
+!to gather roses (life's rose)
+- tìm thú hưởng lạc
+!life is not all roses
+- đời không phải hoa hồng cả, đời sống không phải lúc nào cũng sung sướng an nhàn
+!a path strewn with roses
+- cuộc sống đầy lạc thú
+!there is no rose without a thorn
+- (tục ngữ) không có hoa hồng nào mà không có gai, không có điều gì sướng mà không có cái khổ kèm theo
+!under the rose
+- bí mật âm thầm, kín đáo, lén lút
+*  tính từ
+- hồng, màu hồng
+*  ngoại động từ
+- nhuộm hồng, nhuốm hồng
+=the morning sun rosed the eastern horizon+ mặt trời buổi sáng nhuộm hồng chân trời đằng đông
+*  thời quá khứ của rise
 </t>
   </si>
 </sst>
@@ -1721,7 +1843,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA89061-8BF6-44C5-AC42-B85CC71C0DCE}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -2370,6 +2492,54 @@
         <v>12</v>
       </c>
     </row>
+    <row r="80" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement Register/Login features consist of Forms, Data transmission format and send/receive protocol at Client site
</commit_message>
<xml_diff>
--- a/ClientDictApp/Records/records.xlsx
+++ b/ClientDictApp/Records/records.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4210534-5AC5-4CBC-847B-05CBC55C9BE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E39B69-F73E-49CE-8A8C-0F9530F4A507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5317" yWindow="3733" windowWidth="15951" windowHeight="8230" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
   <si>
     <t>Encoded word</t>
   </si>
@@ -1445,6 +1445,235 @@
 =the morning sun rosed the eastern horizon+ mặt trời buổi sáng nhuộm hồng chân trời đằng đông
 *  thời quá khứ của rise
 </t>
+  </si>
+  <si>
+    <t>story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@story /'stɔ:ri/
+*  danh từ
+- chuyện, câu chuyện
+=they all tell the same story+ họ đều kể một câu chuyện như nhau
+=as the story goes+ người ta nói chuyện rằng
+=but that is another story+ nhưng đó lại là chuyện khác
+- truyện
+=a short story+ truyện ngắn
+- cốt truyện, tình tiết (một truyện, một vở kịch...)
+=he reads only for the story+ anh ta đọc để hiểu cốt truyện thôi
+- tiểu sử, quá khứ (của một người)
+- luây kàng ngốc khoành người nói dối
+=oh you story!+ nói dối!, điêu!
+- (từ cổ,nghĩa cổ) lịch sử, sử học
+*  danh từ
+- (như) storey
+</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@fish /fiʃ/
+*  danh từ
+- cá
+=freshwater fish+ cá nước ngọt
+=salt-water fish+ cá nước mặn
+- cá, món cá
+- (thiên văn học) chòm sao Cá
+- người cắn câu, người bị mồi chài
+- con người gã (có cá tính đặc biệt)
+=a queer fish+ một con người (gã) kỳ quặc
+!all's fish that comes to his net
+- lớn bé, to nhỏ hắn quơ tất
+!to be as drunk as a fish
+- say bí tỉ
+!to be as mute as a fish
+- câm như hến
+!to drink like a fish
+- (xem) drink
+!to feed the fishes
+- chết đuối
+- bị say sóng
+!like a fish out of water
+- (xem) water
+!to have other fish to fly
+- có công việc khác quan trọng hơn
+!he who would catch fish must not mind getting wet
+- muốn ăn cá phải lội nước, muốn ăn hét phải đào giun
+!neither fish, fish, not good red herring
+- môn chẳng ra môn, khoai chẳng ra khoai
+!never fry a fish till it's caught
+- chưa làm vòng chớ vội mong ăn thịt
+!never offer to teach fish to swim
+- chớ nên múa rìu qua mắt thợ
+!a pretty kettle of fish
+- (xem) kettle
+!there's as good fish in the sea as ever came out of it
+- thừa mứa chứa chan, nhiều vô kể
+*  nội động từ
+- đánh cá, câu cá, bắt cá
+=to fish in the sea+ đánh cá ở biển
+- (+ for) tìm, mò (cái gì ở dưới nước)
+- (+ for) câu, moi những điều bí mật
+*  ngoại động từ
+- câu cá ở, đánh cá ở, bắt cá ở
+=to fish a river+ đánh cá ở sông
+- (hàng hải)
+=to fish the anchor+ nhổ neo
+- rút, lấy, kéo, moi
+=to fish something out of water+ kéo cái gì từ dưới nước lên
+- (từ hiếm,nghĩa hiếm) câu (cá), đánh (cá), bắt (cá), tìm (san hô...)
+=to fish a troud+ câu một con cá hồi
+!to fish out
+- đánh hết cá (ở ao...)
+- moi (ý kiến, bí mật)
+!to fish in troubled waters
+- lợi dụng đục nước béo cò
+*  danh từ
+- (hàng hải) miếng gỗ nẹp, miếng sắt nẹp (ở cột buồm, ở chỗ nối)
+- (ngành đường sắt) thanh nối ray ((cũng) fish plate)
+*  ngoại động từ
+- (hàng hải) nẹp (bằng gỗ hay sắt)
+- nối (đường ray) bằng thanh nối ray
+*  danh từ
+- (đánh bài) thẻ (bằng ngà... dùng thay tiền để đánh bài)
+</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"cat","timestamp":"2020-07-09 18:34:00","dest":"0.0.0.1:8080","src":"0.0.0.1:64244"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"dog","timestamp":"2020-07-09 18:34:09","dest":"0.0.0.1:8080","src":"0.0.0.1:64244"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"city","timestamp":"2020-07-09 18:34:51","dest":"0.0.0.1:8080","src":"0.0.0.1:64244"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"big","timestamp":"2020-07-09 18:35:02","dest":"0.0.0.1:8080","src":"0.0.0.1:64244"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@big /big/
+*  tính từ
+- to, lớn
+=a big tree+ cây to
+=big repair+ sửa chữa lớn
+=Big Three+ ba nước lớn
+=Big Five+ năm nước lớn
+- bụng to, có mang, có chửa
+=big with news+ đầy tin, nhiều tin
+- quan trọng
+=a big man+ nhân vật quan trọng
+- hào hiệp, phóng khoáng, rộng lượng
+=he has a big hear+ anh ta là người hào hiệp
+- huênh hoang, khoác lác
+=big words+ những lời nói huênh hoang khoác lác
+=big words+ những lời nói huênh hoang
+!too big for one's boots (breeches, shoes, trousers)
+- (từ lóng) quá tự tin, tự phụ tự mãn; làm bộ làm tịch
+*  phó từ
+- ra vẻ quan trọng, với vẻ quan trọng
+=to look big+ làm ra vẻ quan trọng
+- huênh hoang khoác lác
+=to talk big+ nói huênh hoang, nói phách
+</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"city","timestamp":"2020-07-09 18:35:06","dest":"0.0.0.1:8080","src":"0.0.0.1:64244"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"cat","timestamp":"2020-07-09 18:37:47","dest":"0.0.0.1:8080","src":"0.0.0.1:64244"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"toy","timestamp":"2020-07-09 18:38:01","dest":"0.0.0.1:8080","src":"0.0.0.1:64445"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"cat","timestamp":"2020-07-10 01:13:29","dest":"0.0.0.1:8080","src":"0.0.0.1:60893"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"sent","timestamp":"2020-07-10 01:13:42","dest":"0.0.0.1:8080","src":"0.0.0.1:60893"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@sent /send/
+*  ngoại động từ sent 
+/sent/
+- gửi, sai, phái, cho đi ((cũng) scend)
+=to send word to somebody+ gửi vài chữ cho ai
+=to send a boy a school+ cho một em nhỏ đi học
+- cho, ban cho, phù hộ cho, giáng (trời,  Thượng đế...)
+=send him victorioussend+ trời phụ hộ cho nó thắng trận!
+=to send a drought+ giáng xuống nạn hạn hán
+- bắn ra, làm bốc lên, làm nẩy ra, toả ra
+=to send a ball over the trees+ đá tung quả bóng qua rặng cây
+=to send smoke high in the air+ làm bốc khói lên cao trong không trung
+- đuổi đi, tống đi
+=to send somebody about his business+ tống cổ ai đi
+- làm cho (mê mẩn)
+=to send somebody crazy+ làm ai say mê; (nhạc ja, lóng) làm cho mê li
+- (từ Mỹ,nghĩa Mỹ) hướng tới, đẩy tới
+=your question has sent me to the dictionary+ câu hỏi của anh đã khiến tôi đi tìm từ điển
+*  nội động từ
+- gửi thư, nhắn
+=to send to worn somebody+ gửi thư báo cho ai; gửi thư cảnh cáo ai
+=to send to somebody to take care+ nhắn ai phải cẩn thận
+!to send away
+- gửi đi
+- đuổi di
+!to send after
+- cho đi tìm, cho đuổi theo
+!to send down
+- cho xuống
+- tạm đuổi, đuổi (khỏi trường)
+!to send for
+- gửi đặt mua
+=to send for something+ gửi đặt mua cái gì
+- nhắn đến, cho đi tìm đến, cho mời đến
+=to send for somebody+ nhắn ai tìm đến, cho người mời đến
+=to send for somebody+ nhắn ai đến, cho người mời ai
+!to send forth
+- toả ra, bốc ra (hương thơm, mùi, khói...)
+- nảy ra (lộc non, lá...)
+!to send in
+- nộp, giao (đơn từ...)
+- ghi, đăng (tên...)
+=to send in one's name+ đăng tên (ở kỳ thi)
+!to send off
+- gửi đi (thư, quà) phái (ai) đi (công tác)
+- đuổi đi, tống khứ
+- tiễn đưa, hoan tống
+!to send out
+- gửi đi, phân phát
+- toả ra, bốc ra (hương thơm, mùi, khói...)
+- nảy ra
+=trees send out young leaves+ cây ra lá non
+!to send round
+- chuyền tay, chuyền vòng (vật gì)
+!to send up
+- làm đứng dậy, làm trèo lên
+- (từ Mỹ,nghĩa Mỹ),  (thông tục) kết án tù
+!to send coals to Newcastle
+- (xem) coal
+!to send flying
+- đuổi đi, bắt hối hả ra đi
+- làm cho lảo đảo, đánh bật ra (bằng một cái đòn)
+- làm cho chạy tan tác, làm cho tan tác
+!to send packing
+- đuổi đi, tống cổ đi
+!to send someone to Jericho
+- đuổi ai đi, tống cổ ai đi
+!to send to Coventry
+- phớt lờ, không hợp tác với (ai)
+</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"sent","timestamp":"2020-07-10 01:13:47","dest":"0.0.0.1:8080","src":"0.0.0.1:60893"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"cat","timestamp":"2020-07-10 15:31:39","dest":"0.0.0.1:8080","src":"0.0.0.1:58725"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"toy","timestamp":"2020-07-10 15:31:55","dest":"0.0.0.1:8080","src":"0.0.0.1:58731"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"fish","timestamp":"2020-07-10 15:32:27","dest":"0.0.0.1:8080","src":"0.0.0.1:58725"}</t>
   </si>
 </sst>
 </file>
@@ -1843,7 +2072,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA89061-8BF6-44C5-AC42-B85CC71C0DCE}">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -2540,6 +2769,158 @@
         <v>81</v>
       </c>
     </row>
+    <row r="86" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="360" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix receiveBuffer length bug and fix cryptography framework
</commit_message>
<xml_diff>
--- a/ClientDictApp/Records/records.xlsx
+++ b/ClientDictApp/Records/records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E39B69-F73E-49CE-8A8C-0F9530F4A507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCB2090-9077-44BF-9E5A-330559C90FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5317" yWindow="3733" windowWidth="15951" windowHeight="8230" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="109">
   <si>
     <t>Encoded word</t>
   </si>
@@ -1674,6 +1674,156 @@
   </si>
   <si>
     <t>{"code":300,"content":"fish","timestamp":"2020-07-10 15:32:27","dest":"0.0.0.1:8080","src":"0.0.0.1:58725"}</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"cat","timestamp":"2020-07-14 00:40:28","dest":"0.0.0.1:8080","src":"0.0.0.1:59737"}</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>{"code":300,"content":"long","timestamp":"2020-07-14 00:59:39","dest":"0.0.0.1:8080","src":"0.0.0.1:60492"}</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>skate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@skate /skeit/
+*  danh từ
+- (động vật học) cá đuổi
+*  danh từ
+- (từ Mỹ,nghĩa Mỹ),  (từ lóng) người già ốm
+- người bị khinh rẻ
+*  danh từ
+- lưỡi trượt (ở giày trượt băng)
+*  động từ
+- trượt băng
+!to skate over (on) thin ice
+- nói đến một vấn đề tế nhị
+- ở trong hoàn cảnh nguy hiểm
+</t>
+  </si>
+  <si>
+    <t>strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@strike /straik/
+*  ngoại động từ struck; struck,  stricken
+- đánh, đập
+=to strike one's hand on the table+ đập tay xuống bàn
+=to strike a blow+ đánh một cú
+=to strike hands+ (từ cổ,nghĩa cổ) bắt tay
+=ship strikes rock+ tàu va phải đá
+=tree struck by lightning+ cây bị sét đánh
+=to be stricken with paralysis+ bị tê liệt
+- đánh, điểm
+=to strike sparks (fire, light) out of flint+ đánh đá lửa
+=to strike a match+ đánh diêm
+=clock strikes five+ đồng hồ điểm năm giờ
+- đúc
+=to strike coin+ đúc tiền
+- giật (cá, khi câu)
+- dò đúng, đào đúng (mạch dầu, mạch mỏ...)
+- đánh, tấn công
+- đập vào
+=to strike the ears+ đập vào tai (âm thanh...)
+=a beautiful sight struck my eyes+ một cảnh tượng đẹp đập vào mắt tôi
+=the light struck the window+ ánh sáng rọi vào cửa sổ
+=the idea suddenly struck me+ tôi chợt nảy ra ý nghĩ
+- làm cho phải chú ý, gây ấn tượng
+=what strikes me is his generosity+ điều làm tôi chú ý là tính hào phóng của anh ta
+=how does it strike you?+ anh thấy vấn đề ấy thế nào?
+=it strikes me as absolutely perfect+ tôi cho rằng điều đó tuyệt đối đúng
+- thình lình làm cho; gây (sợ hãi, kinh ngạc...) thình lình
+=to be struck with amazement+ hết sức kinh ngạc
+=to strike terror in someone's heart+ làm cho ai sợi chết khiếp
+- đâm vào, đưa vào; đi vào, tới, đến
+=plant strikes its roots into the soil+ cây đâm rễ xuống đất
+=to strike a track+ đi vào con đường mòn
+=to strike the main road+ tới con đường chính
+- gạt (thùng khi đong thóc...)
+- xoá, bỏ, gạch đi
+=to strike a name out+ xoá một tên đi
+=to strike a word through+ gạch một từ đi
+- hạ (cờ, buồm)
+- bãi, đình (công)
+=to strike work+ bãi công, đình công
+- tính lấy (số trung bình)
+- làm thăng bằng (cái cân)
+- lấy (điệu bộ...)
+- (sân khấu) dỡ và thu dọn (phông); tắt (đèn)
+- dỡ (lều)
+=to strike tents+ dỡ lều, nhổ trại
+*  nội động từ
+- đánh, nhằm đánh
+=to strike at the ball+ nhắm đánh quả bóng
+- gõ, đánh, điểm
+=the hour has struck+ giờ đã điểm
+- bật cháy, chiếu sáng
+=light strikes upon something+ ánh sáng rọi vào một vật gì
+=match will not strike+ diêm không cháy
+- đớp mồi, cắn câu (cá)
+- đâm rễ (cây)
+- tấn công
+- thấm qua
+=cold strikes into marrow+ rét thấm vào tận xương tuỷ
+- đi về phía, hướng về
+=to strike across a field+ vượt qua một cánh đồng
+=to strike to the right+ rẽ về tay phải
+- hạ cờ; hạ cờ đầu hàng, đầu hàng
+=ship strikes+ tàu hạ cờ đầu hàng
+- bãi công, đình công
+!to strike at
+- nhằm vào, đánh vào
+=to strike at the root of something+ doạ triệt cái gì đến tận gốc
+!to strike back
+- đánh trả lại
+- đi trở lại
+!to strike down
+- đánh ngã (đen &amp; bóng)
+!to strike off
+- chặt đứt, xoá bỏ; bớt đi
+!to strike out
+- xoá bỏ, gạch bỏ
+- (+ at) đấm (ai); vung (tay chân khi bơi)
+- lao vụt đi (người bơi...)
+- nghĩ ra, đề ra (kế hoạch...)
+=to strike out a line for oneself+ nghĩ ra được một đường lối độc đáo; to ra có óc sáng tạo
+!to strike through
+- xuyên qua, thấm qua
+!to strike someone dumb
+- (xem) dumb
+!to strike home
+- (xem) home
+!to strike oil
+- đào đúng mạch dầu
+- làm ăn phát đạt
+!to strike up an acquaintance
+- làm quen (với ai)
+!to strike up a tune
+- cất tiếng hát, bắt đầu cử một bản nhạc
+!to strike upon an idea
+- nảy ra một ý kiến
+!to strike it rich
+- dò đúng mạch mỏ... có trữ lượng cao
+- phất
+!to strike in a talk with a suggestion
+- xen vào câu chuyện bằng một lời gợi ý
+!to strike white the iron is hot
+- (xem) iron
+*  danh từ
+- cuộc đình công, cuộc bãi công
+=to go on strike+ bãi công
+=general strike+ cuộc tổng bãi công
+- mẻ đúc
+- sự đột nhiên dò đúng (mạch mỏ)
+- sự phất
+- sự xuất kích
+- que gạt (dấu, thùng đong thóc)
+</t>
   </si>
 </sst>
 </file>
@@ -2072,32 +2222,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA89061-8BF6-44C5-AC42-B85CC71C0DCE}">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="61.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.796875" style="1"/>
+    <col min="3" max="3" width="26.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2105,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2113,7 +2267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2121,7 +2275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2129,7 +2283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2145,7 +2299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2153,7 +2307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2161,7 +2315,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +2323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2177,7 +2331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -2185,7 +2339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2193,7 +2347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -2201,7 +2355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2209,7 +2363,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2857,7 +3011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>92</v>
       </c>
@@ -2865,7 +3019,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>93</v>
       </c>
@@ -2873,7 +3027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>94</v>
       </c>
@@ -2881,7 +3035,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
@@ -2889,7 +3043,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>97</v>
       </c>
@@ -2897,7 +3051,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>98</v>
       </c>
@@ -2905,7 +3059,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>99</v>
       </c>
@@ -2913,12 +3067,64 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename and delete directories, files contain private information
</commit_message>
<xml_diff>
--- a/ClientDictApp/Records/records.xlsx
+++ b/ClientDictApp/Records/records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\Records\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD5F567-FB9D-477B-BC64-13CBBCF407F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFDFD48-C029-45AB-AC78-778A648BCD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
   </bookViews>

</xml_diff>

<commit_message>
Rename namespace and edit README.md
</commit_message>
<xml_diff>
--- a/ClientDictApp/Records/records.xlsx
+++ b/ClientDictApp/Records/records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFDFD48-C029-45AB-AC78-778A648BCD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FD1FC9-3BC6-4B57-A0A2-A6C9AE90D9B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>